<commit_message>
- Agregado de script SQL
</commit_message>
<xml_diff>
--- a/Clase I/TP Clase 1.xlsx
+++ b/Clase I/TP Clase 1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\frocc\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\frocc\Desktop\Repos\LabIII\Clase I\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A48BBAE-35EA-4569-8FD1-7591F31F8E19}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F02EEC17-632B-4A84-B882-41E15FE0312A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{0CAA93F7-BF10-4CFF-83A6-AD1156183841}"/>
   </bookViews>
@@ -290,7 +290,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -303,6 +303,14 @@
       <color rgb="FF008080"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -460,7 +468,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -513,6 +521,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -830,8 +841,8 @@
   <sheetPr codeName="Hoja2"/>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1038,6 +1049,7 @@
       <c r="F10" s="23" t="s">
         <v>25</v>
       </c>
+      <c r="I10" s="26"/>
     </row>
     <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">

</xml_diff>

<commit_message>
- Correcciones al xlsx y al sql
</commit_message>
<xml_diff>
--- a/Clase I/TP Clase 1.xlsx
+++ b/Clase I/TP Clase 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\frocc\Desktop\Repos\LabIII\Clase I\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F02EEC17-632B-4A84-B882-41E15FE0312A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{552E0503-83DD-480D-99F1-789D0E8B72D5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{0CAA93F7-BF10-4CFF-83A6-AD1156183841}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="84">
   <si>
     <t>Socios y actividades</t>
   </si>
@@ -277,13 +277,13 @@
     <t>ID (PK)</t>
   </si>
   <si>
-    <t>Actividad (FK)</t>
-  </si>
-  <si>
     <t>Legajo (PK+FK)</t>
   </si>
   <si>
     <t>Sede (FK)</t>
+  </si>
+  <si>
+    <t>Actividad (PK+FK)</t>
   </si>
 </sst>
 </file>
@@ -468,7 +468,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -522,6 +522,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -842,7 +845,7 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -871,7 +874,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>3</v>
@@ -1073,13 +1076,13 @@
         <v>46</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G13" s="14" t="s">
         <v>77</v>
       </c>
       <c r="H13" s="15" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="I13" s="16" t="s">
         <v>79</v>
@@ -1095,8 +1098,8 @@
       <c r="C14" s="18">
         <v>250</v>
       </c>
-      <c r="D14" s="18" t="s">
-        <v>47</v>
+      <c r="D14" s="18">
+        <v>0</v>
       </c>
       <c r="E14" s="13">
         <v>1</v>
@@ -1121,8 +1124,8 @@
       <c r="C15" s="18">
         <v>450</v>
       </c>
-      <c r="D15" s="18" t="s">
-        <v>48</v>
+      <c r="D15" s="18">
+        <v>1</v>
       </c>
       <c r="E15" s="13">
         <v>3</v>
@@ -1147,8 +1150,8 @@
       <c r="C16" s="18">
         <v>450</v>
       </c>
-      <c r="D16" s="18" t="s">
-        <v>48</v>
+      <c r="D16" s="18">
+        <v>1</v>
       </c>
       <c r="E16" s="13">
         <v>3</v>
@@ -1173,8 +1176,8 @@
       <c r="C17" s="18">
         <v>500</v>
       </c>
-      <c r="D17" s="18" t="s">
-        <v>48</v>
+      <c r="D17" s="18">
+        <v>1</v>
       </c>
       <c r="E17" s="13">
         <v>4</v>
@@ -1199,8 +1202,8 @@
       <c r="C18" s="18">
         <v>1850</v>
       </c>
-      <c r="D18" s="18" t="s">
-        <v>48</v>
+      <c r="D18" s="18">
+        <v>1</v>
       </c>
       <c r="E18" s="13">
         <v>4</v>
@@ -1225,8 +1228,8 @@
       <c r="C19" s="18">
         <v>500</v>
       </c>
-      <c r="D19" s="18" t="s">
-        <v>48</v>
+      <c r="D19" s="18">
+        <v>1</v>
       </c>
       <c r="E19" s="13">
         <v>2</v>
@@ -1251,8 +1254,8 @@
       <c r="C20" s="18">
         <v>100</v>
       </c>
-      <c r="D20" s="18" t="s">
-        <v>47</v>
+      <c r="D20" s="18">
+        <v>0</v>
       </c>
       <c r="E20" s="13">
         <v>1</v>
@@ -1277,8 +1280,8 @@
       <c r="C21" s="18">
         <v>1850</v>
       </c>
-      <c r="D21" s="18" t="s">
-        <v>47</v>
+      <c r="D21" s="18">
+        <v>0</v>
       </c>
       <c r="E21" s="13">
         <v>1</v>
@@ -1303,8 +1306,8 @@
       <c r="C22" s="18">
         <v>1400</v>
       </c>
-      <c r="D22" s="18" t="s">
-        <v>47</v>
+      <c r="D22" s="18">
+        <v>0</v>
       </c>
       <c r="E22" s="13">
         <v>1</v>
@@ -1329,8 +1332,8 @@
       <c r="C23" s="21">
         <v>500</v>
       </c>
-      <c r="D23" s="21" t="s">
-        <v>47</v>
+      <c r="D23" s="21">
+        <v>0</v>
       </c>
       <c r="E23" s="23">
         <v>2</v>
@@ -1350,7 +1353,7 @@
       <c r="B24" s="24"/>
       <c r="C24" s="24"/>
       <c r="D24" s="24"/>
-      <c r="E24" s="24"/>
+      <c r="E24" s="27"/>
       <c r="G24" s="17">
         <v>7000</v>
       </c>
@@ -1545,7 +1548,7 @@
   <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G10"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>